<commit_message>
Reorganizacion y poblacion final
</commit_message>
<xml_diff>
--- a/docs/Documentación Base de datos.xlsx
+++ b/docs/Documentación Base de datos.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Documentación" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -968,6 +968,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -993,42 +1029,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1371,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82:F94"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1392,31 +1392,31 @@
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="35"/>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="37"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -1595,31 +1595,31 @@
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="39"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="50"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
     </row>
     <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
       <c r="G19" t="s">
         <v>159</v>
       </c>
@@ -2073,31 +2073,31 @@
       <c r="A36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="44"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="33" t="s">
+      <c r="B37" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="35"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="47"/>
     </row>
     <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="37"/>
-      <c r="D38" s="38"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="50"/>
     </row>
     <row r="39" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
@@ -2304,31 +2304,31 @@
       <c r="A54" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="31"/>
-      <c r="D54" s="32"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="44"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="33" t="s">
+      <c r="B55" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="34"/>
-      <c r="D55" s="35"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="47"/>
     </row>
     <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="36" t="s">
+      <c r="B56" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="37"/>
-      <c r="D56" s="38"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="50"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
@@ -2447,31 +2447,31 @@
       <c r="A66" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="30" t="s">
+      <c r="B66" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="31"/>
-      <c r="D66" s="32"/>
+      <c r="C66" s="43"/>
+      <c r="D66" s="44"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B67" s="33" t="s">
+      <c r="B67" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="C67" s="34"/>
-      <c r="D67" s="35"/>
+      <c r="C67" s="46"/>
+      <c r="D67" s="47"/>
     </row>
     <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B68" s="36" t="s">
+      <c r="B68" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C68" s="37"/>
-      <c r="D68" s="38"/>
+      <c r="C68" s="49"/>
+      <c r="D68" s="50"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
@@ -2648,11 +2648,11 @@
       <c r="A82" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B82" s="30" t="s">
+      <c r="B82" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="C82" s="31"/>
-      <c r="D82" s="32"/>
+      <c r="C82" s="43"/>
+      <c r="D82" s="44"/>
       <c r="F82" t="s">
         <v>181</v>
       </c>
@@ -2661,11 +2661,11 @@
       <c r="A83" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B83" s="33" t="s">
+      <c r="B83" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="C83" s="34"/>
-      <c r="D83" s="35"/>
+      <c r="C83" s="46"/>
+      <c r="D83" s="47"/>
       <c r="F83" t="s">
         <v>180</v>
       </c>
@@ -2674,11 +2674,11 @@
       <c r="A84" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B84" s="36" t="s">
+      <c r="B84" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C84" s="37"/>
-      <c r="D84" s="38"/>
+      <c r="C84" s="49"/>
+      <c r="D84" s="50"/>
       <c r="F84" t="s">
         <v>179</v>
       </c>
@@ -2803,12 +2803,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
     <mergeCell ref="B82:D82"/>
     <mergeCell ref="B83:D83"/>
     <mergeCell ref="B84:D84"/>
@@ -2821,6 +2815,12 @@
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="B66:D66"/>
     <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>